<commit_message>
DODANE GS DLA PROFILI
TYLKO OPERACJA SPAWANIA
</commit_message>
<xml_diff>
--- a/tabela_mapowania.xlsx
+++ b/tabela_mapowania.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\QNAP-ENERGO\Technologia\2023\40.1033_45621033\INTEGRA_ZLOZENIE-40.1033_45621033\IMPORTERY\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\QNAP-ENERGO\Technologia\2023\39.0772__45620772\INTEGRA_ZLOZENIE-39_0772A\IMPORTERY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEE54546-57FE-4847-BE90-9065A7D55348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED1460AE-EE82-46D7-96F7-0EAC3C93CD82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="51">
   <si>
     <t>typ</t>
   </si>
@@ -574,10 +574,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P24"/>
+  <dimension ref="A1:P25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C16" sqref="C16:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1063,36 +1063,24 @@
       <c r="P15" s="1"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>34</v>
+      <c r="A16" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>36</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
@@ -1105,13 +1093,13 @@
         <v>33</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>19</v>
@@ -1119,10 +1107,18 @@
       <c r="F17" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
+      <c r="G17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
@@ -1134,39 +1130,27 @@
       <c r="A18" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>39</v>
+      <c r="B18" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H18" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I18" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>36</v>
-      </c>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
@@ -1177,7 +1161,7 @@
         <v>33</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>40</v>
@@ -1219,7 +1203,7 @@
         <v>33</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>40</v>
@@ -1261,26 +1245,38 @@
         <v>33</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>44</v>
+        <v>40</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="E21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="H21" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
+      <c r="I21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
@@ -1291,7 +1287,7 @@
         <v>33</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>43</v>
@@ -1317,30 +1313,60 @@
       <c r="P22" s="1"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="A23" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="7" t="s">
-        <v>49</v>
+      <c r="B23" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>47</v>
-      </c>
+      <c r="F23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>33</v>
       </c>
       <c r="B24" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C25" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D25" s="6" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ELEMENT DODANE + ZŁOŻENIE 3
NA ŻÓŁTO SZYBKI DOBOR MARSZRUT
</commit_message>
<xml_diff>
--- a/tabela_mapowania.xlsx
+++ b/tabela_mapowania.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\QNAP-ENERGO\Technologia\2023\52. 2158_45622158 - 6FB\PK\INTEGRA_ZLOZENIE-52_BL5_MARSZRUTY\IMPORTERY\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\QNAP-ENERGO\Technologia\2024\01. 2891_Dynamix\INTEGRA_ZLOZENIE-01,02_2891_2894_DYNAMIX\IMPORTERY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BADEC910-2041-40EF-9D6A-064D2A6EC7B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D1F257-F292-494E-9ECA-460D694A8C38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-90" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="62">
   <si>
     <t>typ</t>
   </si>
@@ -207,6 +207,21 @@
   </si>
   <si>
     <t>Giecie</t>
+  </si>
+  <si>
+    <t>ELEMENT</t>
+  </si>
+  <si>
+    <t>Przygotowanie_do_produkcji</t>
+  </si>
+  <si>
+    <t>LUZEM</t>
+  </si>
+  <si>
+    <t>Elementy_Luzem</t>
+  </si>
+  <si>
+    <t>ZŁOŻENIE3</t>
   </si>
 </sst>
 </file>
@@ -251,12 +266,18 @@
       <charset val="238"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -286,7 +307,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -295,12 +316,36 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -581,16 +626,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P35"/>
+  <dimension ref="A1:P55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32:D32"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53:D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.77734375" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" style="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
@@ -611,7 +656,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -661,7 +706,7 @@
       <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="4">
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -695,7 +740,7 @@
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>23</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -729,7 +774,7 @@
       <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -763,7 +808,7 @@
       <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>25</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -789,7 +834,7 @@
       <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>28</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -815,7 +860,7 @@
       <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -849,7 +894,7 @@
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>30</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -875,7 +920,7 @@
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="8" t="s">
         <v>37</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -901,7 +946,7 @@
       <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="4" t="s">
         <v>31</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -927,7 +972,7 @@
       <c r="A11" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="4" t="s">
         <v>30</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -953,7 +998,7 @@
       <c r="A12" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="4" t="s">
         <v>31</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -979,7 +1024,7 @@
       <c r="A13" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="8" t="s">
         <v>37</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -1005,7 +1050,7 @@
       <c r="A14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="4">
         <v>0</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -1039,7 +1084,7 @@
       <c r="A15" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -1073,7 +1118,7 @@
       <c r="A16" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="4" t="s">
         <v>25</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -1099,7 +1144,7 @@
       <c r="A17" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="8" t="s">
         <v>34</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -1137,7 +1182,7 @@
       <c r="A18" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="8" t="s">
         <v>37</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -1167,7 +1212,7 @@
       <c r="A19" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="4" t="s">
         <v>39</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -1209,7 +1254,7 @@
       <c r="A20" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="4" t="s">
         <v>42</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -1251,7 +1296,7 @@
       <c r="A21" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="4" t="s">
         <v>46</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -1293,13 +1338,13 @@
       <c r="A22" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="4" t="s">
         <v>43</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="4" t="s">
         <v>44</v>
       </c>
       <c r="E22" s="1" t="s">
@@ -1323,13 +1368,13 @@
       <c r="A23" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="4" t="s">
         <v>45</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="4" t="s">
         <v>44</v>
       </c>
       <c r="E23" s="1" t="s">
@@ -1350,10 +1395,10 @@
       <c r="P23" s="1"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="4" t="s">
         <v>49</v>
       </c>
       <c r="C24" s="1" t="s">
@@ -1362,50 +1407,50 @@
       <c r="D24" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="7"/>
-      <c r="L24" s="7"/>
-      <c r="M24" s="7"/>
-      <c r="N24" s="7"/>
-      <c r="O24" s="7"/>
-      <c r="P24" s="7"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="6"/>
+      <c r="P24" s="6"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="7"/>
-      <c r="K25" s="7"/>
-      <c r="L25" s="7"/>
-      <c r="M25" s="7"/>
-      <c r="N25" s="7"/>
-      <c r="O25" s="7"/>
-      <c r="P25" s="7"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="6"/>
+      <c r="M25" s="6"/>
+      <c r="N25" s="6"/>
+      <c r="O25" s="6"/>
+      <c r="P25" s="6"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="4" t="s">
         <v>51</v>
       </c>
       <c r="C26" s="1" t="s">
@@ -1414,182 +1459,820 @@
       <c r="D26" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="7"/>
-      <c r="J26" s="7"/>
-      <c r="K26" s="7"/>
-      <c r="L26" s="7"/>
-      <c r="M26" s="7"/>
-      <c r="N26" s="7"/>
-      <c r="O26" s="7"/>
-      <c r="P26" s="7"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
+      <c r="N26" s="6"/>
+      <c r="O26" s="6"/>
+      <c r="P26" s="6"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C27" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D27" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="E27" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="F27" s="7" t="s">
+      <c r="F27" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
-      <c r="J27" s="7"/>
-      <c r="K27" s="7"/>
-      <c r="L27" s="7"/>
-      <c r="M27" s="7"/>
-      <c r="N27" s="7"/>
-      <c r="O27" s="7"/>
-      <c r="P27" s="7"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="6"/>
+      <c r="M27" s="6"/>
+      <c r="N27" s="6"/>
+      <c r="O27" s="6"/>
+      <c r="P27" s="6"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="C28" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="D28" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E28" s="7" t="s">
+      <c r="E28" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="F28" s="7" t="s">
+      <c r="F28" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="H28" s="7"/>
-      <c r="I28" s="7"/>
-      <c r="J28" s="7"/>
-      <c r="K28" s="7"/>
-      <c r="L28" s="7"/>
-      <c r="M28" s="7"/>
-      <c r="N28" s="7"/>
-      <c r="O28" s="7"/>
-      <c r="P28" s="7"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="6"/>
+      <c r="M28" s="6"/>
+      <c r="N28" s="6"/>
+      <c r="O28" s="6"/>
+      <c r="P28" s="6"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C29" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="D29" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E29" s="7" t="s">
+      <c r="E29" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="F29" s="7" t="s">
+      <c r="F29" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="H29" s="7"/>
-      <c r="I29" s="7"/>
-      <c r="J29" s="7"/>
-      <c r="K29" s="7"/>
-      <c r="L29" s="7"/>
-      <c r="M29" s="7"/>
-      <c r="N29" s="7"/>
-      <c r="O29" s="7"/>
-      <c r="P29" s="7"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="6"/>
+      <c r="M29" s="6"/>
+      <c r="N29" s="6"/>
+      <c r="O29" s="6"/>
+      <c r="P29" s="6"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="C30" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="D30" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E30" s="7" t="s">
+      <c r="E30" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="F30" s="7" t="s">
+      <c r="F30" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
-      <c r="J30" s="7"/>
-      <c r="K30" s="7"/>
-      <c r="L30" s="7"/>
-      <c r="M30" s="7"/>
-      <c r="N30" s="7"/>
-      <c r="O30" s="7"/>
-      <c r="P30" s="7"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="6"/>
+      <c r="L30" s="6"/>
+      <c r="M30" s="6"/>
+      <c r="N30" s="6"/>
+      <c r="O30" s="6"/>
+      <c r="P30" s="6"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="C31" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D31" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
-      <c r="J31" s="7"/>
-      <c r="K31" s="7"/>
-      <c r="L31" s="7"/>
-      <c r="M31" s="7"/>
-      <c r="N31" s="7"/>
-      <c r="O31" s="7"/>
-      <c r="P31" s="7"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
+      <c r="L31" s="6"/>
+      <c r="M31" s="6"/>
+      <c r="N31" s="6"/>
+      <c r="O31" s="6"/>
+      <c r="P31" s="6"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="15">
         <v>0</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="C32" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D32" s="7" t="s">
+      <c r="D32" s="6" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" s="2"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" s="2"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" s="2"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="6"/>
+      <c r="L32" s="6"/>
+      <c r="M32" s="6"/>
+      <c r="N32" s="6"/>
+      <c r="O32" s="6"/>
+      <c r="P32" s="6"/>
+    </row>
+    <row r="33" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B33" s="11">
+        <v>0</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="12"/>
+      <c r="J33" s="12"/>
+      <c r="K33" s="16"/>
+      <c r="L33" s="16"/>
+      <c r="M33" s="16"/>
+      <c r="N33" s="16"/>
+      <c r="O33" s="16"/>
+      <c r="P33" s="16"/>
+    </row>
+    <row r="34" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="12"/>
+      <c r="J34" s="12"/>
+      <c r="K34" s="16"/>
+      <c r="L34" s="16"/>
+      <c r="M34" s="16"/>
+      <c r="N34" s="16"/>
+      <c r="O34" s="16"/>
+      <c r="P34" s="16"/>
+    </row>
+    <row r="35" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D35" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="12"/>
+      <c r="I35" s="12"/>
+      <c r="J35" s="12"/>
+      <c r="K35" s="16"/>
+      <c r="L35" s="16"/>
+      <c r="M35" s="16"/>
+      <c r="N35" s="16"/>
+      <c r="O35" s="16"/>
+      <c r="P35" s="16"/>
+    </row>
+    <row r="36" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D36" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="12"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="12"/>
+      <c r="K36" s="16"/>
+      <c r="L36" s="16"/>
+      <c r="M36" s="16"/>
+      <c r="N36" s="16"/>
+      <c r="O36" s="16"/>
+      <c r="P36" s="16"/>
+    </row>
+    <row r="37" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="12"/>
+      <c r="I37" s="12"/>
+      <c r="J37" s="12"/>
+      <c r="K37" s="16"/>
+      <c r="L37" s="16"/>
+      <c r="M37" s="16"/>
+      <c r="N37" s="16"/>
+      <c r="O37" s="16"/>
+      <c r="P37" s="16"/>
+    </row>
+    <row r="38" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="12"/>
+      <c r="I38" s="12"/>
+      <c r="J38" s="12"/>
+      <c r="K38" s="16"/>
+      <c r="L38" s="16"/>
+      <c r="M38" s="16"/>
+      <c r="N38" s="16"/>
+      <c r="O38" s="16"/>
+      <c r="P38" s="16"/>
+    </row>
+    <row r="39" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E39" s="12"/>
+      <c r="F39" s="12"/>
+      <c r="G39" s="12"/>
+      <c r="H39" s="12"/>
+      <c r="I39" s="12"/>
+      <c r="J39" s="12"/>
+      <c r="K39" s="16"/>
+      <c r="L39" s="16"/>
+      <c r="M39" s="16"/>
+      <c r="N39" s="16"/>
+      <c r="O39" s="16"/>
+      <c r="P39" s="16"/>
+    </row>
+    <row r="40" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B40" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D40" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E40" s="12"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="12"/>
+      <c r="H40" s="12"/>
+      <c r="I40" s="12"/>
+      <c r="J40" s="12"/>
+      <c r="K40" s="16"/>
+      <c r="L40" s="16"/>
+      <c r="M40" s="16"/>
+      <c r="N40" s="16"/>
+      <c r="O40" s="16"/>
+      <c r="P40" s="16"/>
+    </row>
+    <row r="41" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B41" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D41" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E41" s="12"/>
+      <c r="F41" s="12"/>
+      <c r="G41" s="12"/>
+      <c r="H41" s="12"/>
+      <c r="I41" s="12"/>
+      <c r="J41" s="12"/>
+      <c r="K41" s="16"/>
+      <c r="L41" s="16"/>
+      <c r="M41" s="16"/>
+      <c r="N41" s="16"/>
+      <c r="O41" s="16"/>
+      <c r="P41" s="16"/>
+    </row>
+    <row r="42" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B42" s="11">
+        <v>0</v>
+      </c>
+      <c r="C42" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D42" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="E42" s="16"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="16"/>
+      <c r="H42" s="16"/>
+      <c r="I42" s="16"/>
+      <c r="J42" s="16"/>
+      <c r="K42" s="16"/>
+      <c r="L42" s="16"/>
+      <c r="M42" s="16"/>
+      <c r="N42" s="16"/>
+      <c r="O42" s="16"/>
+      <c r="P42" s="16"/>
+    </row>
+    <row r="43" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C43" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D43" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="E43" s="16"/>
+      <c r="F43" s="16"/>
+      <c r="G43" s="16"/>
+      <c r="H43" s="16"/>
+      <c r="I43" s="16"/>
+      <c r="J43" s="16"/>
+      <c r="K43" s="16"/>
+      <c r="L43" s="16"/>
+      <c r="M43" s="16"/>
+      <c r="N43" s="16"/>
+      <c r="O43" s="16"/>
+      <c r="P43" s="16"/>
+    </row>
+    <row r="44" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B44" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C44" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D44" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="E44" s="16"/>
+      <c r="F44" s="16"/>
+      <c r="G44" s="16"/>
+      <c r="H44" s="16"/>
+      <c r="I44" s="16"/>
+      <c r="J44" s="16"/>
+      <c r="K44" s="16"/>
+      <c r="L44" s="16"/>
+      <c r="M44" s="16"/>
+      <c r="N44" s="16"/>
+      <c r="O44" s="16"/>
+      <c r="P44" s="16"/>
+    </row>
+    <row r="45" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C45" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D45" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="E45" s="16"/>
+      <c r="F45" s="16"/>
+      <c r="G45" s="16"/>
+      <c r="H45" s="16"/>
+      <c r="I45" s="16"/>
+      <c r="J45" s="16"/>
+      <c r="K45" s="16"/>
+      <c r="L45" s="16"/>
+      <c r="M45" s="16"/>
+      <c r="N45" s="16"/>
+      <c r="O45" s="16"/>
+      <c r="P45" s="16"/>
+    </row>
+    <row r="46" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B46" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C46" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D46" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E46" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F46" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G46" s="16"/>
+      <c r="H46" s="16"/>
+      <c r="I46" s="16"/>
+      <c r="J46" s="16"/>
+      <c r="K46" s="16"/>
+      <c r="L46" s="16"/>
+      <c r="M46" s="16"/>
+      <c r="N46" s="16"/>
+      <c r="O46" s="16"/>
+      <c r="P46" s="16"/>
+    </row>
+    <row r="47" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B47" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
+      <c r="H47" s="16"/>
+      <c r="I47" s="16"/>
+      <c r="J47" s="16"/>
+      <c r="K47" s="16"/>
+      <c r="L47" s="16"/>
+      <c r="M47" s="16"/>
+      <c r="N47" s="16"/>
+      <c r="O47" s="16"/>
+      <c r="P47" s="16"/>
+    </row>
+    <row r="48" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B48" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D48" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E48" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F48" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G48" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="H48" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="I48" s="16"/>
+      <c r="J48" s="16"/>
+      <c r="K48" s="16"/>
+      <c r="L48" s="16"/>
+      <c r="M48" s="16"/>
+      <c r="N48" s="16"/>
+      <c r="O48" s="16"/>
+      <c r="P48" s="16"/>
+    </row>
+    <row r="49" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B49" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C49" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D49" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E49" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F49" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G49" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="H49" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="I49" s="16"/>
+      <c r="J49" s="16"/>
+      <c r="K49" s="16"/>
+      <c r="L49" s="16"/>
+      <c r="M49" s="16"/>
+      <c r="N49" s="16"/>
+      <c r="O49" s="16"/>
+      <c r="P49" s="16"/>
+    </row>
+    <row r="50" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B50" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C50" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D50" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E50" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F50" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G50" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="H50" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="I50" s="16"/>
+      <c r="J50" s="16"/>
+      <c r="K50" s="16"/>
+      <c r="L50" s="16"/>
+      <c r="M50" s="16"/>
+      <c r="N50" s="16"/>
+      <c r="O50" s="16"/>
+      <c r="P50" s="16"/>
+    </row>
+    <row r="51" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B51" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C51" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D51" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E51" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F51" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G51" s="16"/>
+      <c r="H51" s="16"/>
+      <c r="I51" s="16"/>
+      <c r="J51" s="16"/>
+      <c r="K51" s="16"/>
+      <c r="L51" s="16"/>
+      <c r="M51" s="16"/>
+      <c r="N51" s="16"/>
+      <c r="O51" s="16"/>
+      <c r="P51" s="16"/>
+    </row>
+    <row r="52" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B52" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C52" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D52" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E52" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F52" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G52" s="16"/>
+      <c r="H52" s="16"/>
+      <c r="I52" s="16"/>
+      <c r="J52" s="16"/>
+      <c r="K52" s="16"/>
+      <c r="L52" s="16"/>
+      <c r="M52" s="16"/>
+      <c r="N52" s="16"/>
+      <c r="O52" s="16"/>
+      <c r="P52" s="16"/>
+    </row>
+    <row r="53" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B53" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C53" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D53" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="E53" s="16"/>
+      <c r="F53" s="16"/>
+      <c r="G53" s="16"/>
+      <c r="H53" s="16"/>
+      <c r="I53" s="16"/>
+      <c r="J53" s="16"/>
+      <c r="K53" s="16"/>
+      <c r="L53" s="16"/>
+      <c r="M53" s="16"/>
+      <c r="N53" s="16"/>
+      <c r="O53" s="16"/>
+      <c r="P53" s="16"/>
+    </row>
+    <row r="54" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B54" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C54" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D54" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E54" s="16"/>
+      <c r="F54" s="16"/>
+      <c r="G54" s="16"/>
+      <c r="H54" s="16"/>
+      <c r="I54" s="16"/>
+      <c r="J54" s="16"/>
+      <c r="K54" s="16"/>
+      <c r="L54" s="16"/>
+      <c r="M54" s="16"/>
+      <c r="N54" s="16"/>
+      <c r="O54" s="16"/>
+      <c r="P54" s="16"/>
+    </row>
+    <row r="55" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B55" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C55" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D55" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E55" s="16"/>
+      <c r="F55" s="16"/>
+      <c r="G55" s="16"/>
+      <c r="H55" s="16"/>
+      <c r="I55" s="16"/>
+      <c r="J55" s="16"/>
+      <c r="K55" s="16"/>
+      <c r="L55" s="16"/>
+      <c r="M55" s="16"/>
+      <c r="N55" s="16"/>
+      <c r="O55" s="16"/>
+      <c r="P55" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
cm - czarny montaz + malowanie
</commit_message>
<xml_diff>
--- a/tabela_mapowania.xlsx
+++ b/tabela_mapowania.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\QNAP-ENERGO\Technologia\2025\09_6412-45646412(3FB)\INTEGRA_ZLOZENIE-09_6412\IMPORTERY\MARSZRUTA2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\QNAP-ENERGO\Technologia\2025\12_8152\INTEGRA_ZLOZENIE-12_8152\IMPORTERY\MARSZRUTA2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DEF7711-63C2-4160-8157-91F88A40B862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93A8BCCC-FE34-43A5-8B14-B0E6E1814D21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-90" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="93">
   <si>
     <t>typ</t>
   </si>
@@ -307,18 +307,35 @@
   </si>
   <si>
     <t>KJ</t>
+  </si>
+  <si>
+    <t>CM</t>
+  </si>
+  <si>
+    <t>MALARNIA</t>
+  </si>
+  <si>
+    <t>Malowanie</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -448,69 +465,74 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -791,10 +813,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P72"/>
+  <dimension ref="A1:P75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1095,17 +1117,37 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
+    <row r="10" spans="1:16" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>92</v>
+      </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
@@ -1113,25 +1155,17 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A11" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="B11" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
+    <row r="11" spans="1:16" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="30"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
@@ -1139,21 +1173,9 @@
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A12" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="B12" s="22" t="s">
-        <v>81</v>
-      </c>
-      <c r="C12" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="D12" s="23" t="s">
-        <v>82</v>
-      </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
+    <row r="12" spans="1:16" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="29"/>
+      <c r="B12" s="28"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
@@ -1166,18 +1188,10 @@
       <c r="P12" s="1"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A13" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>76</v>
-      </c>
+      <c r="A13" s="1"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -1192,11 +1206,11 @@
       <c r="P13" s="1"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A14" s="26" t="s">
+      <c r="A14" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="B14" s="15" t="s">
-        <v>64</v>
+      <c r="B14" s="21" t="s">
+        <v>47</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>70</v>
@@ -1204,13 +1218,9 @@
       <c r="D14" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="E14" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="G14" s="27"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -1222,10 +1232,18 @@
       <c r="P14" s="1"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
+      <c r="A15" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>82</v>
+      </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -1240,10 +1258,18 @@
       <c r="P15" s="1"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
+      <c r="A16" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>76</v>
+      </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
@@ -1258,13 +1284,25 @@
       <c r="P16" s="1"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A17" s="1"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
+      <c r="A17" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="G17" s="27"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
@@ -1276,30 +1314,14 @@
       <c r="P17" s="1"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B18" s="4">
-        <v>0</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="A18" s="1"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
@@ -1310,30 +1332,14 @@
       <c r="P18" s="1"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="A19" s="1"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
@@ -1344,30 +1350,14 @@
       <c r="P19" s="1"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="A20" s="1"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
@@ -1381,19 +1371,27 @@
       <c r="A21" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>24</v>
+      <c r="B21" s="4">
+        <v>0</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
@@ -1408,18 +1406,26 @@
         <v>61</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
@@ -1434,7 +1440,7 @@
         <v>61</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>16</v>
@@ -1468,7 +1474,7 @@
         <v>61</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>25</v>
@@ -1493,14 +1499,14 @@
       <c r="A25" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B25" s="8" t="s">
-        <v>35</v>
+      <c r="B25" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -1520,18 +1526,26 @@
         <v>61</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
@@ -1542,8 +1556,8 @@
       <c r="P26" s="1"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A27" s="3" t="s">
-        <v>62</v>
+      <c r="A27" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>29</v>
@@ -1568,17 +1582,17 @@
       <c r="P27" s="1"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>30</v>
+      <c r="A28" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>35</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
@@ -1594,17 +1608,17 @@
       <c r="P28" s="1"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>35</v>
+      <c r="A29" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -1623,27 +1637,19 @@
       <c r="A30" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B30" s="4">
-        <v>0</v>
+      <c r="B30" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>21</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
@@ -1658,26 +1664,18 @@
         <v>62</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>21</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
@@ -1691,14 +1689,14 @@
       <c r="A32" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B32" s="4" t="s">
-        <v>24</v>
+      <c r="B32" s="8" t="s">
+        <v>35</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
@@ -1714,11 +1712,11 @@
       <c r="P32" s="1"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>32</v>
+      <c r="A33" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B33" s="4">
+        <v>0</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>16</v>
@@ -1738,12 +1736,8 @@
       <c r="H33" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I33" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J33" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
@@ -1752,17 +1746,17 @@
       <c r="P33" s="1"/>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>35</v>
+      <c r="A34" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>18</v>
@@ -1770,8 +1764,12 @@
       <c r="F34" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
+      <c r="G34" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
@@ -1782,42 +1780,26 @@
       <c r="P34" s="1"/>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
-        <v>63</v>
+      <c r="A35" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I35" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J35" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K35" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L35" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
       <c r="M35" s="1"/>
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
@@ -1827,39 +1809,35 @@
       <c r="A36" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B36" s="4" t="s">
-        <v>40</v>
+      <c r="B36" s="8" t="s">
+        <v>32</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K36" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L36" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
       <c r="M36" s="1"/>
       <c r="N36" s="1"/>
       <c r="O36" s="1"/>
@@ -1869,39 +1847,27 @@
       <c r="A37" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B37" s="4" t="s">
-        <v>44</v>
+      <c r="B37" s="8" t="s">
+        <v>35</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H37" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I37" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J37" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K37" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L37" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
       <c r="M37" s="1"/>
       <c r="N37" s="1"/>
       <c r="O37" s="1"/>
@@ -1912,26 +1878,38 @@
         <v>63</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="E38" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G38" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F38" s="1" t="s">
+      <c r="H38" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
-      <c r="K38" s="1"/>
-      <c r="L38" s="1"/>
+      <c r="I38" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L38" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
       <c r="O38" s="1"/>
@@ -1942,26 +1920,38 @@
         <v>63</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="E39" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G39" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F39" s="1" t="s">
+      <c r="H39" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
-      <c r="K39" s="1"/>
-      <c r="L39" s="1"/>
+      <c r="I39" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L39" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="M39" s="1"/>
       <c r="N39" s="1"/>
       <c r="O39" s="1"/>
@@ -1972,98 +1962,118 @@
         <v>63</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C40" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G40" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D40" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E40" s="6"/>
-      <c r="F40" s="6"/>
-      <c r="G40" s="6"/>
-      <c r="H40" s="6"/>
-      <c r="I40" s="6"/>
-      <c r="J40" s="6"/>
-      <c r="K40" s="6"/>
-      <c r="L40" s="6"/>
-      <c r="M40" s="6"/>
-      <c r="N40" s="6"/>
-      <c r="O40" s="6"/>
-      <c r="P40" s="6"/>
+      <c r="H40" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L40" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M40" s="1"/>
+      <c r="N40" s="1"/>
+      <c r="O40" s="1"/>
+      <c r="P40" s="1"/>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
-      <c r="G41" s="6"/>
-      <c r="H41" s="6"/>
-      <c r="I41" s="6"/>
-      <c r="J41" s="6"/>
-      <c r="K41" s="6"/>
-      <c r="L41" s="6"/>
-      <c r="M41" s="6"/>
-      <c r="N41" s="6"/>
-      <c r="O41" s="6"/>
-      <c r="P41" s="6"/>
+        <v>41</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+      <c r="L41" s="1"/>
+      <c r="M41" s="1"/>
+      <c r="N41" s="1"/>
+      <c r="O41" s="1"/>
+      <c r="P41" s="1"/>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C42" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E42" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="F42" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E42" s="6"/>
-      <c r="F42" s="6"/>
-      <c r="G42" s="6"/>
-      <c r="H42" s="6"/>
-      <c r="I42" s="6"/>
-      <c r="J42" s="6"/>
-      <c r="K42" s="6"/>
-      <c r="L42" s="6"/>
-      <c r="M42" s="6"/>
-      <c r="N42" s="6"/>
-      <c r="O42" s="6"/>
-      <c r="P42" s="6"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1"/>
+      <c r="L42" s="1"/>
+      <c r="M42" s="1"/>
+      <c r="N42" s="1"/>
+      <c r="O42" s="1"/>
+      <c r="P42" s="1"/>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C43" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D43" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E43" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F43" s="6" t="s">
-        <v>54</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
       <c r="G43" s="6"/>
       <c r="H43" s="6"/>
       <c r="I43" s="6"/>
@@ -2077,23 +2087,19 @@
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D44" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E44" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F44" s="6" t="s">
-        <v>54</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
       <c r="G44" s="6"/>
       <c r="H44" s="6"/>
       <c r="I44" s="6"/>
@@ -2107,23 +2113,19 @@
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D45" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E45" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F45" s="6" t="s">
-        <v>54</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
       <c r="G45" s="6"/>
       <c r="H45" s="6"/>
       <c r="I45" s="6"/>
@@ -2140,7 +2142,7 @@
         <v>50</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C46" s="6" t="s">
         <v>51</v>
@@ -2170,7 +2172,7 @@
         <v>50</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C47" s="6" t="s">
         <v>51</v>
@@ -2178,8 +2180,12 @@
       <c r="D47" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E47" s="6"/>
-      <c r="F47" s="6"/>
+      <c r="E47" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>54</v>
+      </c>
       <c r="G47" s="6"/>
       <c r="H47" s="6"/>
       <c r="I47" s="6"/>
@@ -2195,8 +2201,8 @@
       <c r="A48" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B48" s="15">
-        <v>0</v>
+      <c r="B48" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="C48" s="6" t="s">
         <v>51</v>
@@ -2204,8 +2210,12 @@
       <c r="D48" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E48" s="6"/>
-      <c r="F48" s="6"/>
+      <c r="E48" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>54</v>
+      </c>
       <c r="G48" s="6"/>
       <c r="H48" s="6"/>
       <c r="I48" s="6"/>
@@ -2217,96 +2227,100 @@
       <c r="O48" s="6"/>
       <c r="P48" s="6"/>
     </row>
-    <row r="49" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="B49" s="11">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G49" s="6"/>
+      <c r="H49" s="6"/>
+      <c r="I49" s="6"/>
+      <c r="J49" s="6"/>
+      <c r="K49" s="6"/>
+      <c r="L49" s="6"/>
+      <c r="M49" s="6"/>
+      <c r="N49" s="6"/>
+      <c r="O49" s="6"/>
+      <c r="P49" s="6"/>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A50" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E50" s="6"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="6"/>
+      <c r="H50" s="6"/>
+      <c r="I50" s="6"/>
+      <c r="J50" s="6"/>
+      <c r="K50" s="6"/>
+      <c r="L50" s="6"/>
+      <c r="M50" s="6"/>
+      <c r="N50" s="6"/>
+      <c r="O50" s="6"/>
+      <c r="P50" s="6"/>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A51" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B51" s="15">
         <v>0</v>
       </c>
-      <c r="C49" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D49" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="E49" s="12"/>
-      <c r="F49" s="12"/>
-      <c r="G49" s="12"/>
-      <c r="H49" s="12"/>
-      <c r="I49" s="12"/>
-      <c r="J49" s="12"/>
-      <c r="K49" s="16"/>
-      <c r="L49" s="16"/>
-      <c r="M49" s="16"/>
-      <c r="N49" s="16"/>
-      <c r="O49" s="16"/>
-      <c r="P49" s="16"/>
-    </row>
-    <row r="50" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="B50" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C50" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D50" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="E50" s="12"/>
-      <c r="F50" s="12"/>
-      <c r="G50" s="12"/>
-      <c r="H50" s="12"/>
-      <c r="I50" s="12"/>
-      <c r="J50" s="12"/>
-      <c r="K50" s="16"/>
-      <c r="L50" s="16"/>
-      <c r="M50" s="16"/>
-      <c r="N50" s="16"/>
-      <c r="O50" s="16"/>
-      <c r="P50" s="16"/>
-    </row>
-    <row r="51" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="B51" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C51" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D51" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="E51" s="12"/>
-      <c r="F51" s="12"/>
-      <c r="G51" s="12"/>
-      <c r="H51" s="12"/>
-      <c r="I51" s="12"/>
-      <c r="J51" s="12"/>
-      <c r="K51" s="16"/>
-      <c r="L51" s="16"/>
-      <c r="M51" s="16"/>
-      <c r="N51" s="16"/>
-      <c r="O51" s="16"/>
-      <c r="P51" s="16"/>
+      <c r="C51" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="6"/>
+      <c r="H51" s="6"/>
+      <c r="I51" s="6"/>
+      <c r="J51" s="6"/>
+      <c r="K51" s="6"/>
+      <c r="L51" s="6"/>
+      <c r="M51" s="6"/>
+      <c r="N51" s="6"/>
+      <c r="O51" s="6"/>
+      <c r="P51" s="6"/>
     </row>
     <row r="52" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B52" s="11" t="s">
-        <v>24</v>
+      <c r="B52" s="11">
+        <v>0</v>
       </c>
       <c r="C52" s="12" t="s">
         <v>25</v>
       </c>
       <c r="D52" s="12" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="E52" s="12"/>
       <c r="F52" s="12"/>
@@ -2326,13 +2340,13 @@
         <v>55</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C53" s="12" t="s">
         <v>25</v>
       </c>
       <c r="D53" s="12" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="E53" s="12"/>
       <c r="F53" s="12"/>
@@ -2352,7 +2366,7 @@
         <v>55</v>
       </c>
       <c r="B54" s="11" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C54" s="12" t="s">
         <v>25</v>
@@ -2378,7 +2392,7 @@
         <v>55</v>
       </c>
       <c r="B55" s="11" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C55" s="12" t="s">
         <v>25</v>
@@ -2403,14 +2417,14 @@
       <c r="A56" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B56" s="14" t="s">
-        <v>35</v>
+      <c r="B56" s="11" t="s">
+        <v>27</v>
       </c>
       <c r="C56" s="12" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="D56" s="12" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="E56" s="12"/>
       <c r="F56" s="12"/>
@@ -2430,13 +2444,13 @@
         <v>55</v>
       </c>
       <c r="B57" s="11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C57" s="12" t="s">
         <v>25</v>
       </c>
       <c r="D57" s="12" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="E57" s="12"/>
       <c r="F57" s="12"/>
@@ -2453,23 +2467,23 @@
     </row>
     <row r="58" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="B58" s="11">
-        <v>0</v>
-      </c>
-      <c r="C58" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="D58" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="E58" s="16"/>
-      <c r="F58" s="16"/>
-      <c r="G58" s="16"/>
-      <c r="H58" s="16"/>
-      <c r="I58" s="16"/>
-      <c r="J58" s="16"/>
+        <v>55</v>
+      </c>
+      <c r="B58" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C58" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D58" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E58" s="12"/>
+      <c r="F58" s="12"/>
+      <c r="G58" s="12"/>
+      <c r="H58" s="12"/>
+      <c r="I58" s="12"/>
+      <c r="J58" s="12"/>
       <c r="K58" s="16"/>
       <c r="L58" s="16"/>
       <c r="M58" s="16"/>
@@ -2479,23 +2493,23 @@
     </row>
     <row r="59" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="B59" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C59" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="D59" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="E59" s="16"/>
-      <c r="F59" s="16"/>
-      <c r="G59" s="16"/>
-      <c r="H59" s="16"/>
-      <c r="I59" s="16"/>
-      <c r="J59" s="16"/>
+        <v>55</v>
+      </c>
+      <c r="B59" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C59" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D59" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E59" s="12"/>
+      <c r="F59" s="12"/>
+      <c r="G59" s="12"/>
+      <c r="H59" s="12"/>
+      <c r="I59" s="12"/>
+      <c r="J59" s="12"/>
       <c r="K59" s="16"/>
       <c r="L59" s="16"/>
       <c r="M59" s="16"/>
@@ -2505,23 +2519,23 @@
     </row>
     <row r="60" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B60" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C60" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="D60" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="E60" s="16"/>
-      <c r="F60" s="16"/>
-      <c r="G60" s="16"/>
-      <c r="H60" s="16"/>
-      <c r="I60" s="16"/>
-      <c r="J60" s="16"/>
+        <v>30</v>
+      </c>
+      <c r="C60" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D60" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E60" s="12"/>
+      <c r="F60" s="12"/>
+      <c r="G60" s="12"/>
+      <c r="H60" s="12"/>
+      <c r="I60" s="12"/>
+      <c r="J60" s="12"/>
       <c r="K60" s="16"/>
       <c r="L60" s="16"/>
       <c r="M60" s="16"/>
@@ -2533,8 +2547,8 @@
       <c r="A61" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B61" s="11" t="s">
-        <v>28</v>
+      <c r="B61" s="11">
+        <v>0</v>
       </c>
       <c r="C61" s="16" t="s">
         <v>20</v>
@@ -2557,23 +2571,19 @@
     </row>
     <row r="62" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="B62" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C62" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B62" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C62" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="D62" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="E62" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="F62" s="12" t="s">
-        <v>34</v>
-      </c>
+      <c r="D62" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E62" s="16"/>
+      <c r="F62" s="16"/>
       <c r="G62" s="16"/>
       <c r="H62" s="16"/>
       <c r="I62" s="16"/>
@@ -2587,23 +2597,19 @@
     </row>
     <row r="63" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="B63" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="C63" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="D63" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="E63" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="F63" s="12" t="s">
-        <v>19</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="B63" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C63" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D63" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E63" s="16"/>
+      <c r="F63" s="16"/>
       <c r="G63" s="16"/>
       <c r="H63" s="16"/>
       <c r="I63" s="16"/>
@@ -2617,29 +2623,21 @@
     </row>
     <row r="64" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B64" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C64" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D64" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="E64" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C64" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="F64" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="G64" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="H64" s="12" t="s">
-        <v>34</v>
-      </c>
+      <c r="D64" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E64" s="16"/>
+      <c r="F64" s="16"/>
+      <c r="G64" s="16"/>
+      <c r="H64" s="16"/>
       <c r="I64" s="16"/>
       <c r="J64" s="16"/>
       <c r="K64" s="16"/>
@@ -2653,27 +2651,23 @@
       <c r="A65" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="B65" s="11" t="s">
-        <v>40</v>
+      <c r="B65" s="14" t="s">
+        <v>32</v>
       </c>
       <c r="C65" s="12" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="D65" s="12" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="E65" s="12" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="F65" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="G65" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="H65" s="12" t="s">
         <v>34</v>
       </c>
+      <c r="G65" s="16"/>
+      <c r="H65" s="16"/>
       <c r="I65" s="16"/>
       <c r="J65" s="16"/>
       <c r="K65" s="16"/>
@@ -2687,27 +2681,23 @@
       <c r="A66" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="B66" s="11" t="s">
-        <v>44</v>
+      <c r="B66" s="14" t="s">
+        <v>35</v>
       </c>
       <c r="C66" s="12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D66" s="12" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E66" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F66" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="G66" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="H66" s="12" t="s">
-        <v>34</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="G66" s="16"/>
+      <c r="H66" s="16"/>
       <c r="I66" s="16"/>
       <c r="J66" s="16"/>
       <c r="K66" s="16"/>
@@ -2722,22 +2712,26 @@
         <v>59</v>
       </c>
       <c r="B67" s="11" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C67" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="D67" s="11" t="s">
-        <v>42</v>
+        <v>38</v>
+      </c>
+      <c r="D67" s="12" t="s">
+        <v>39</v>
       </c>
       <c r="E67" s="12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F67" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="G67" s="16"/>
-      <c r="H67" s="16"/>
+        <v>21</v>
+      </c>
+      <c r="G67" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H67" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="I67" s="16"/>
       <c r="J67" s="16"/>
       <c r="K67" s="16"/>
@@ -2752,22 +2746,26 @@
         <v>59</v>
       </c>
       <c r="B68" s="11" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C68" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="D68" s="11" t="s">
-        <v>42</v>
+        <v>38</v>
+      </c>
+      <c r="D68" s="12" t="s">
+        <v>39</v>
       </c>
       <c r="E68" s="12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F68" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="G68" s="16"/>
-      <c r="H68" s="16"/>
+        <v>21</v>
+      </c>
+      <c r="G68" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H68" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="I68" s="16"/>
       <c r="J68" s="16"/>
       <c r="K68" s="16"/>
@@ -2782,18 +2780,26 @@
         <v>59</v>
       </c>
       <c r="B69" s="11" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C69" s="12" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="D69" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="E69" s="16"/>
-      <c r="F69" s="16"/>
-      <c r="G69" s="16"/>
-      <c r="H69" s="16"/>
+        <v>39</v>
+      </c>
+      <c r="E69" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F69" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G69" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H69" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="I69" s="16"/>
       <c r="J69" s="16"/>
       <c r="K69" s="16"/>
@@ -2808,16 +2814,20 @@
         <v>59</v>
       </c>
       <c r="B70" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="C70" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="D70" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="E70" s="16"/>
-      <c r="F70" s="16"/>
+        <v>41</v>
+      </c>
+      <c r="C70" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D70" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E70" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F70" s="12" t="s">
+        <v>19</v>
+      </c>
       <c r="G70" s="16"/>
       <c r="H70" s="16"/>
       <c r="I70" s="16"/>
@@ -2834,16 +2844,20 @@
         <v>59</v>
       </c>
       <c r="B71" s="11" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C71" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D71" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E71" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D71" s="12" t="s">
+      <c r="F71" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E71" s="16"/>
-      <c r="F71" s="16"/>
       <c r="G71" s="16"/>
       <c r="H71" s="16"/>
       <c r="I71" s="16"/>
@@ -2855,17 +2869,95 @@
       <c r="O71" s="16"/>
       <c r="P71" s="16"/>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A72" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B72" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C72" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D72" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E72" s="16"/>
+      <c r="F72" s="16"/>
+      <c r="G72" s="16"/>
+      <c r="H72" s="16"/>
+      <c r="I72" s="16"/>
+      <c r="J72" s="16"/>
+      <c r="K72" s="16"/>
+      <c r="L72" s="16"/>
+      <c r="M72" s="16"/>
+      <c r="N72" s="16"/>
+      <c r="O72" s="16"/>
+      <c r="P72" s="16"/>
+    </row>
+    <row r="73" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B73" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C73" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D73" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="E73" s="16"/>
+      <c r="F73" s="16"/>
+      <c r="G73" s="16"/>
+      <c r="H73" s="16"/>
+      <c r="I73" s="16"/>
+      <c r="J73" s="16"/>
+      <c r="K73" s="16"/>
+      <c r="L73" s="16"/>
+      <c r="M73" s="16"/>
+      <c r="N73" s="16"/>
+      <c r="O73" s="16"/>
+      <c r="P73" s="16"/>
+    </row>
+    <row r="74" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B74" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C74" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D74" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E74" s="16"/>
+      <c r="F74" s="16"/>
+      <c r="G74" s="16"/>
+      <c r="H74" s="16"/>
+      <c r="I74" s="16"/>
+      <c r="J74" s="16"/>
+      <c r="K74" s="16"/>
+      <c r="L74" s="16"/>
+      <c r="M74" s="16"/>
+      <c r="N74" s="16"/>
+      <c r="O74" s="16"/>
+      <c r="P74" s="16"/>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A75" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B72" s="11" t="s">
+      <c r="B75" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C72" s="12" t="s">
+      <c r="C75" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D72" s="12" t="s">
+      <c r="D75" s="12" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
dodano M - malowanie
</commit_message>
<xml_diff>
--- a/tabela_mapowania.xlsx
+++ b/tabela_mapowania.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\QNAP-ENERGO\Technologia\2025\09_6412-45646412(3FB)\INTEGRA_ZLOZENIE-09_6412Biały Montaż (BM)\IMPORTERY\MARSZRUTA2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\QNAP-ENERGO\Technologia\BAZA\TABELA MAPOWANIA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6714E148-63F1-45B8-B994-F41C03D0EB7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{155AC399-0CE0-4281-ABE2-E5B479F09B80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-90" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="stare_NIEAKTUALNE" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MARSZRUTY_NOWE!$B$1:$N$23</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MARSZRUTY_NOWE!$B$1:$N$24</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="102">
   <si>
     <t>typ</t>
   </si>
@@ -343,18 +343,29 @@
   </si>
   <si>
     <t>wstrzymane</t>
+  </si>
+  <si>
+    <t>M</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -534,80 +545,79 @@
   </cellStyleXfs>
   <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -616,25 +626,28 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -917,10 +930,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q23"/>
+  <dimension ref="A1:Q24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="D4" sqref="D4:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -948,7 +961,7 @@
       <c r="A1" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="41" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="7" t="s">
@@ -999,7 +1012,7 @@
     </row>
     <row r="2" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16"/>
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="42" t="s">
         <v>31</v>
       </c>
       <c r="C2" s="21" t="s">
@@ -1038,7 +1051,7 @@
     </row>
     <row r="3" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="42" t="s">
         <v>31</v>
       </c>
       <c r="C3" s="22" t="s">
@@ -1077,24 +1090,24 @@
     </row>
     <row r="4" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16"/>
-      <c r="B4" s="43" t="s">
+      <c r="B4" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="E4" s="16" t="s">
-        <v>67</v>
+      <c r="C4" s="53" t="s">
+        <v>101</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>86</v>
       </c>
       <c r="F4" s="16"/>
       <c r="G4" s="16"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
       <c r="L4" s="12"/>
       <c r="M4" s="12"/>
       <c r="N4" s="12"/>
@@ -1104,24 +1117,20 @@
     </row>
     <row r="5" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="22" t="s">
-        <v>92</v>
+      <c r="C5" s="24" t="s">
+        <v>64</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="G5" s="16" t="s">
         <v>67</v>
       </c>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
       <c r="H5" s="12"/>
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
@@ -1133,13 +1142,13 @@
       <c r="P5" s="12"/>
       <c r="Q5" s="12"/>
     </row>
-    <row r="6" spans="1:17" s="13" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16"/>
-      <c r="B6" s="44" t="s">
+      <c r="B6" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="25" t="s">
-        <v>47</v>
+      <c r="C6" s="22" t="s">
+        <v>92</v>
       </c>
       <c r="D6" s="16" t="s">
         <v>69</v>
@@ -1147,8 +1156,12 @@
       <c r="E6" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
+      <c r="F6" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>67</v>
+      </c>
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
@@ -1162,17 +1175,17 @@
     </row>
     <row r="7" spans="1:17" s="13" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16"/>
-      <c r="B7" s="44" t="s">
+      <c r="B7" s="43" t="s">
         <v>31</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
@@ -1187,44 +1200,28 @@
       <c r="P7" s="12"/>
       <c r="Q7" s="12"/>
     </row>
-    <row r="8" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" s="13" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16"/>
       <c r="B8" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="22" t="s">
-        <v>90</v>
+      <c r="C8" s="25" t="s">
+        <v>79</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="G8" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="H8" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="I8" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="J8" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="K8" s="23" t="s">
-        <v>91</v>
-      </c>
-      <c r="L8" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="M8" s="16" t="s">
-        <v>67</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
       <c r="N8" s="12"/>
       <c r="O8" s="12"/>
       <c r="P8" s="12"/>
@@ -1232,11 +1229,11 @@
     </row>
     <row r="9" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16"/>
-      <c r="B9" s="43" t="s">
+      <c r="B9" s="42" t="s">
         <v>31</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D9" s="16" t="s">
         <v>65</v>
@@ -1262,87 +1259,99 @@
       <c r="K9" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="L9" s="23" t="s">
-        <v>87</v>
-      </c>
-      <c r="M9" s="23" t="s">
-        <v>86</v>
+      <c r="L9" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="M9" s="16" t="s">
+        <v>67</v>
       </c>
       <c r="N9" s="12"/>
       <c r="O9" s="12"/>
       <c r="P9" s="12"/>
       <c r="Q9" s="12"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A10" s="6"/>
-    </row>
-    <row r="11" spans="1:17" s="29" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="27"/>
-      <c r="B11" s="45" t="s">
+    <row r="10" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="16"/>
+      <c r="B10" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C10" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="H10" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="I10" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="J10" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="K10" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="L10" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="M10" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="N10" s="12"/>
+      <c r="O10" s="12"/>
+      <c r="P10" s="12"/>
+      <c r="Q10" s="12"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A11" s="6"/>
+    </row>
+    <row r="12" spans="1:17" s="28" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="27"/>
+      <c r="B12" s="44" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="26" t="s">
         <v>81</v>
-      </c>
-      <c r="D11" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="E11" s="28" t="s">
-        <v>89</v>
-      </c>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="27"/>
-      <c r="J11" s="27"/>
-      <c r="K11" s="27"/>
-      <c r="P11" s="30"/>
-      <c r="Q11" s="30"/>
-    </row>
-    <row r="12" spans="1:17" s="29" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="27"/>
-      <c r="B12" s="46" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="53" t="s">
-        <v>48</v>
       </c>
       <c r="D12" s="27" t="s">
         <v>65</v>
       </c>
       <c r="E12" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="27"/>
+      <c r="P12" s="29"/>
+      <c r="Q12" s="29"/>
+    </row>
+    <row r="13" spans="1:17" s="28" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="27"/>
+      <c r="B13" s="45" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="52" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" s="27" t="s">
         <v>19</v>
-      </c>
-      <c r="F12" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="G12" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="H12" s="30"/>
-      <c r="I12" s="30"/>
-      <c r="J12" s="30"/>
-      <c r="K12" s="30"/>
-      <c r="L12" s="30"/>
-      <c r="M12" s="30"/>
-      <c r="N12" s="30"/>
-      <c r="O12" s="30"/>
-      <c r="P12" s="30"/>
-      <c r="Q12" s="30"/>
-    </row>
-    <row r="13" spans="1:17" s="29" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="27"/>
-      <c r="B13" s="47" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="31" t="s">
-        <v>84</v>
-      </c>
-      <c r="D13" s="27" t="s">
-        <v>71</v>
-      </c>
-      <c r="E13" s="27" t="s">
-        <v>82</v>
       </c>
       <c r="F13" s="27" t="s">
         <v>83</v>
@@ -1350,256 +1359,268 @@
       <c r="G13" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="H13" s="30"/>
-      <c r="I13" s="30"/>
-      <c r="J13" s="30"/>
-      <c r="K13" s="30"/>
-      <c r="L13" s="30"/>
-      <c r="M13" s="30"/>
-      <c r="N13" s="30"/>
-      <c r="O13" s="30"/>
-      <c r="P13" s="30"/>
-      <c r="Q13" s="30"/>
-    </row>
-    <row r="14" spans="1:17" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="6"/>
-      <c r="B14" s="48"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
-      <c r="Q14" s="1"/>
-    </row>
-    <row r="15" spans="1:17" s="32" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="34"/>
-      <c r="B15" s="49" t="s">
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="29"/>
+      <c r="K13" s="29"/>
+      <c r="L13" s="29"/>
+      <c r="M13" s="29"/>
+      <c r="N13" s="29"/>
+      <c r="O13" s="29"/>
+      <c r="P13" s="29"/>
+      <c r="Q13" s="29"/>
+    </row>
+    <row r="14" spans="1:17" s="28" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="27"/>
+      <c r="B14" s="46" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="E14" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="F14" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="G14" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="29"/>
+      <c r="K14" s="29"/>
+      <c r="L14" s="29"/>
+      <c r="M14" s="29"/>
+      <c r="N14" s="29"/>
+      <c r="O14" s="29"/>
+      <c r="P14" s="29"/>
+      <c r="Q14" s="29"/>
+    </row>
+    <row r="15" spans="1:17" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="6"/>
+      <c r="B15" s="47"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+    </row>
+    <row r="16" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="33"/>
+      <c r="B16" s="48" t="s">
         <v>75</v>
       </c>
-      <c r="C15" s="33" t="s">
+      <c r="C16" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="D15" s="34" t="s">
+      <c r="D16" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="34" t="s">
+      <c r="E16" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="35"/>
-      <c r="I15" s="35"/>
-      <c r="J15" s="35"/>
-      <c r="K15" s="35"/>
-      <c r="L15" s="35"/>
-      <c r="M15" s="35"/>
-      <c r="N15" s="35"/>
-      <c r="O15" s="35"/>
-      <c r="P15" s="35"/>
-      <c r="Q15" s="35"/>
-    </row>
-    <row r="16" spans="1:17" s="32" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="34"/>
-      <c r="B16" s="49" t="s">
+      <c r="F16" s="34"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="34"/>
+      <c r="L16" s="34"/>
+      <c r="M16" s="34"/>
+      <c r="N16" s="34"/>
+      <c r="O16" s="34"/>
+      <c r="P16" s="34"/>
+      <c r="Q16" s="34"/>
+    </row>
+    <row r="17" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="33"/>
+      <c r="B17" s="48" t="s">
         <v>75</v>
       </c>
-      <c r="C16" s="36" t="s">
+      <c r="C17" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="D16" s="34" t="s">
+      <c r="D17" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="34" t="s">
+      <c r="E17" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="F16" s="35"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
-      <c r="K16" s="35"/>
-      <c r="L16" s="35"/>
-      <c r="M16" s="35"/>
-      <c r="N16" s="35"/>
-      <c r="O16" s="35"/>
-      <c r="P16" s="35"/>
-      <c r="Q16" s="35"/>
-    </row>
-    <row r="17" spans="1:17" s="32" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="34"/>
-      <c r="B17" s="50" t="s">
-        <v>75</v>
-      </c>
-      <c r="C17" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="D17" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="E17" s="34" t="s">
-        <v>70</v>
-      </c>
-      <c r="F17" s="34" t="s">
-        <v>64</v>
-      </c>
-      <c r="G17" s="34" t="s">
-        <v>67</v>
-      </c>
-      <c r="H17" s="38"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
-      <c r="K17" s="35"/>
-      <c r="L17" s="35"/>
-      <c r="M17" s="35"/>
-      <c r="N17" s="35"/>
-      <c r="O17" s="35"/>
-      <c r="P17" s="35"/>
-      <c r="Q17" s="35"/>
-    </row>
-    <row r="18" spans="1:17" s="32" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="34" t="s">
-        <v>100</v>
-      </c>
+      <c r="F17" s="34"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="34"/>
+      <c r="J17" s="34"/>
+      <c r="K17" s="34"/>
+      <c r="L17" s="34"/>
+      <c r="M17" s="34"/>
+      <c r="N17" s="34"/>
+      <c r="O17" s="34"/>
+      <c r="P17" s="34"/>
+      <c r="Q17" s="34"/>
+    </row>
+    <row r="18" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="33"/>
       <c r="B18" s="49" t="s">
         <v>75</v>
       </c>
-      <c r="C18" s="39" t="s">
+      <c r="C18" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="E18" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="F18" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="G18" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="H18" s="37"/>
+      <c r="I18" s="34"/>
+      <c r="J18" s="34"/>
+      <c r="K18" s="34"/>
+      <c r="L18" s="34"/>
+      <c r="M18" s="34"/>
+      <c r="N18" s="34"/>
+      <c r="O18" s="34"/>
+      <c r="P18" s="34"/>
+      <c r="Q18" s="34"/>
+    </row>
+    <row r="19" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="33" t="s">
+        <v>100</v>
+      </c>
+      <c r="B19" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="D18" s="40" t="s">
+      <c r="D19" s="39" t="s">
         <v>78</v>
       </c>
-      <c r="E18" s="40" t="s">
+      <c r="E19" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
-      <c r="K18" s="35"/>
-      <c r="L18" s="35"/>
-      <c r="M18" s="35"/>
-      <c r="N18" s="35"/>
-      <c r="O18" s="35"/>
-      <c r="P18" s="35"/>
-      <c r="Q18" s="35"/>
-    </row>
-    <row r="19" spans="1:17" s="32" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="34"/>
-      <c r="B19" s="51" t="s">
+      <c r="F19" s="34"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="34"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="34"/>
+      <c r="K19" s="34"/>
+      <c r="L19" s="34"/>
+      <c r="M19" s="34"/>
+      <c r="N19" s="34"/>
+      <c r="O19" s="34"/>
+      <c r="P19" s="34"/>
+      <c r="Q19" s="34"/>
+    </row>
+    <row r="20" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="33"/>
+      <c r="B20" s="50" t="s">
         <v>75</v>
       </c>
-      <c r="C19" s="41" t="s">
+      <c r="C20" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="D19" s="34" t="s">
+      <c r="D20" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="E19" s="34" t="s">
+      <c r="E20" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="F19" s="35" t="s">
+      <c r="F20" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="G19" s="35" t="s">
+      <c r="G20" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="H19" s="35"/>
-      <c r="I19" s="35"/>
-      <c r="J19" s="35"/>
-      <c r="K19" s="35"/>
-      <c r="L19" s="35"/>
-      <c r="M19" s="35"/>
-      <c r="N19" s="35"/>
-      <c r="O19" s="35"/>
-      <c r="P19" s="35"/>
-      <c r="Q19" s="35"/>
-    </row>
-    <row r="20" spans="1:17" s="32" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="34" t="s">
+      <c r="H20" s="34"/>
+      <c r="I20" s="34"/>
+      <c r="J20" s="34"/>
+      <c r="K20" s="34"/>
+      <c r="L20" s="34"/>
+      <c r="M20" s="34"/>
+      <c r="N20" s="34"/>
+      <c r="O20" s="34"/>
+      <c r="P20" s="34"/>
+      <c r="Q20" s="34"/>
+    </row>
+    <row r="21" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="33" t="s">
         <v>100</v>
       </c>
-      <c r="B20" s="51" t="s">
+      <c r="B21" s="50" t="s">
         <v>75</v>
       </c>
-      <c r="C20" s="41" t="s">
+      <c r="C21" s="40" t="s">
         <v>97</v>
       </c>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="35"/>
-      <c r="G20" s="35"/>
-      <c r="H20" s="35"/>
-      <c r="I20" s="35"/>
-      <c r="J20" s="35"/>
-      <c r="K20" s="35"/>
-      <c r="L20" s="35"/>
-      <c r="M20" s="35"/>
-      <c r="N20" s="35"/>
-      <c r="O20" s="35"/>
-      <c r="P20" s="35"/>
-      <c r="Q20" s="35"/>
-    </row>
-    <row r="21" spans="1:17" s="32" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="34" t="s">
+      <c r="D21" s="33"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="34"/>
+      <c r="I21" s="34"/>
+      <c r="J21" s="34"/>
+      <c r="K21" s="34"/>
+      <c r="L21" s="34"/>
+      <c r="M21" s="34"/>
+      <c r="N21" s="34"/>
+      <c r="O21" s="34"/>
+      <c r="P21" s="34"/>
+      <c r="Q21" s="34"/>
+    </row>
+    <row r="22" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="33" t="s">
         <v>100</v>
       </c>
-      <c r="B21" s="51" t="s">
+      <c r="B22" s="50" t="s">
         <v>75</v>
       </c>
-      <c r="C21" s="41" t="s">
+      <c r="C22" s="40" t="s">
         <v>98</v>
       </c>
-      <c r="D21" s="34"/>
-      <c r="E21" s="34"/>
-      <c r="F21" s="35"/>
-      <c r="G21" s="35"/>
-      <c r="H21" s="35"/>
-      <c r="I21" s="35"/>
-      <c r="J21" s="35"/>
-      <c r="K21" s="35"/>
-      <c r="L21" s="35"/>
-      <c r="M21" s="35"/>
-      <c r="N21" s="35"/>
-      <c r="O21" s="35"/>
-      <c r="P21" s="35"/>
-      <c r="Q21" s="35"/>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A22" s="6"/>
-      <c r="B22" s="52"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="1"/>
-      <c r="O22" s="1"/>
-      <c r="P22" s="1"/>
-      <c r="Q22" s="1"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="33"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="34"/>
+      <c r="H22" s="34"/>
+      <c r="I22" s="34"/>
+      <c r="J22" s="34"/>
+      <c r="K22" s="34"/>
+      <c r="L22" s="34"/>
+      <c r="M22" s="34"/>
+      <c r="N22" s="34"/>
+      <c r="O22" s="34"/>
+      <c r="P22" s="34"/>
+      <c r="Q22" s="34"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="6"/>
-      <c r="B23" s="42"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
+      <c r="B23" s="51"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
@@ -1613,8 +1634,27 @@
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
     </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A24" s="6"/>
+      <c r="B24" s="41"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+    </row>
   </sheetData>
-  <autoFilter ref="B1:N80" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="B1:N81" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>